<commit_message>
AutoCommit_9 января 2024 г. 12:46:54_SibNout2023
</commit_message>
<xml_diff>
--- a/Отчетность/2023-2024_2ОИБАС1022_Операционные системы_I семестр.xlsx
+++ b/Отчетность/2023-2024_2ОИБАС1022_Операционные системы_I семестр.xlsx
@@ -516,7 +516,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -574,37 +574,44 @@
         <v>2</v>
       </c>
       <c r="D3">
+        <f>SUM(D4:D34)</f>
         <v>26</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <f>SUM(F3:I3)</f>
+        <v>26</v>
       </c>
       <c r="F3">
-        <v>13</v>
+        <f>SUM(F4:F31)</f>
+        <v>10</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <f>SUM(G4:G31)</f>
+        <v>7</v>
       </c>
       <c r="H3">
+        <f>SUM(H4:H31)</f>
         <v>9</v>
       </c>
       <c r="I3">
+        <f>SUM(I4:I31)</f>
         <v>0</v>
       </c>
       <c r="J3">
+        <f>SUM(J4:J31)</f>
         <v>0</v>
       </c>
       <c r="K3" s="5">
-        <f>((F3*F2)+(G3*G2)+(H3*H2)+(I3*I2))/E3</f>
-        <v>4.1333333333333337</v>
+        <f>((F3*5)+(G3*4)+(H3*3)+(I3*2))/E3</f>
+        <v>4.0384615384615383</v>
       </c>
       <c r="L3" s="6">
         <f>((F3+G3)/D3)</f>
-        <v>0.80769230769230771</v>
+        <v>0.65384615384615385</v>
       </c>
       <c r="M3" s="6">
         <f>(F3+G3+H3)/D3</f>
-        <v>1.1538461538461537</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -616,6 +623,29 @@
       </c>
       <c r="C4" s="2">
         <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f>IF(F$2=$C4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:J4" si="0">IF(G$2=$C4,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -628,6 +658,29 @@
       <c r="C5" s="2">
         <v>3</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:J29" si="1">IF(F$2=$C5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -639,6 +692,29 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -650,6 +726,29 @@
       <c r="C7" s="2">
         <v>3</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -661,6 +760,29 @@
       <c r="C8" s="2">
         <v>5</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -672,6 +794,29 @@
       <c r="C9" s="2">
         <v>4</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -683,6 +828,29 @@
       <c r="C10" s="2">
         <v>5</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -694,6 +862,29 @@
       <c r="C11" s="2">
         <v>3</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -705,6 +896,29 @@
       <c r="C12" s="2">
         <v>5</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -716,6 +930,29 @@
       <c r="C13" s="2">
         <v>3</v>
       </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -727,6 +964,29 @@
       <c r="C14" s="2">
         <v>5</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -738,6 +998,29 @@
       <c r="C15" s="2">
         <v>3</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -749,8 +1032,31 @@
       <c r="C16" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -760,8 +1066,31 @@
       <c r="C17" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -771,8 +1100,31 @@
       <c r="C18" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -782,8 +1134,31 @@
       <c r="C19" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -793,8 +1168,31 @@
       <c r="C20" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -804,8 +1202,31 @@
       <c r="C21" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -815,8 +1236,31 @@
       <c r="C22" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -826,8 +1270,31 @@
       <c r="C23" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -837,8 +1304,31 @@
       <c r="C24" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -848,8 +1338,31 @@
       <c r="C25" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -859,8 +1372,31 @@
       <c r="C26" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -870,8 +1406,31 @@
       <c r="C27" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -881,8 +1440,31 @@
       <c r="C28" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -892,14 +1474,49 @@
       <c r="C29" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C30" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <conditionalFormatting sqref="F4:J29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_9 января 2024 г. 12:55:26_SibNout2023
</commit_message>
<xml_diff>
--- a/Отчетность/2023-2024_2ОИБАС1022_Операционные системы_I семестр.xlsx
+++ b/Отчетность/2023-2024_2ОИБАС1022_Операционные системы_I семестр.xlsx
@@ -516,7 +516,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3:M3"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -602,15 +602,15 @@
         <v>0</v>
       </c>
       <c r="K3" s="5">
-        <f>((F3*5)+(G3*4)+(H3*3)+(I3*2))/E3</f>
+        <f>(F3*5+G3*4+H3*3+I3*2)/E3</f>
         <v>4.0384615384615383</v>
       </c>
       <c r="L3" s="6">
-        <f>((F3+G3)/D3)</f>
+        <f>(F3+G3)/E3</f>
         <v>0.65384615384615385</v>
       </c>
       <c r="M3" s="6">
-        <f>(F3+G3+H3)/D3</f>
+        <f>(F3+G3+H3)/E3</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>